<commit_message>
Credenziali altri componenti del gruppo
</commit_message>
<xml_diff>
--- a/03.Informazioni progetto IS.xlsx
+++ b/03.Informazioni progetto IS.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\arman\OneDrive\Desktop\Is\CinemaNow\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F011A14-C0CA-4970-9DA9-C4DBEB0EA4F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE94622D-4E28-49CD-85B3-4F8EB29F7E92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="progetto" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="23">
   <si>
     <t>Progetto</t>
   </si>
@@ -78,14 +78,44 @@
     <t>a.vigliotti5@studenti.unisa.it</t>
   </si>
   <si>
-    <t>CinemaNow</t>
+    <t>0512120565</t>
+  </si>
+  <si>
+    <t>Iovane</t>
+  </si>
+  <si>
+    <t>Emanuele</t>
+  </si>
+  <si>
+    <t>e.iovane2@studenti.unisa.it</t>
+  </si>
+  <si>
+    <t>0512117751</t>
+  </si>
+  <si>
+    <t>Caiazzo</t>
+  </si>
+  <si>
+    <t>Antonio</t>
+  </si>
+  <si>
+    <t>a.caiazzo38@studenti.unisa.it</t>
+  </si>
+  <si>
+    <t>https://github.com/emanueleivn/CinemaNow</t>
+  </si>
+  <si>
+    <t>WebApp per prenotazioni posti a sedere nelle sale cinema</t>
+  </si>
+  <si>
+    <t>CineNow</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -132,14 +162,6 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -197,7 +219,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -205,7 +227,6 @@
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="36"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="37">
     <cellStyle name="Collegamento ipertestuale" xfId="1" builtinId="8" hidden="1"/>
@@ -581,17 +602,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="200" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="200" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="15.69921875" customWidth="1"/>
     <col min="2" max="2" width="47.69921875" customWidth="1"/>
-    <col min="3" max="3" width="36" customWidth="1"/>
+    <col min="3" max="3" width="50.8984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
@@ -603,6 +624,17 @@
       </c>
       <c r="C1" s="3" t="s">
         <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>
@@ -614,14 +646,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E249"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="200" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="200" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="11.69921875" customWidth="1"/>
-    <col min="2" max="4" width="17" customWidth="1"/>
+    <col min="2" max="3" width="17" customWidth="1"/>
+    <col min="4" max="4" width="25.59765625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="27.5" customWidth="1"/>
   </cols>
   <sheetData>
@@ -643,11 +676,21 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A2" s="2"/>
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
+      <c r="A2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
@@ -662,16 +705,26 @@
       <c r="D3" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="E3" s="7" t="s">
-        <v>12</v>
+      <c r="E3" s="1" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4" s="2"/>
-      <c r="B4" s="1"/>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
+      <c r="A4" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="2"/>
@@ -2391,6 +2444,8 @@
   </sheetData>
   <hyperlinks>
     <hyperlink ref="D3" r:id="rId1" xr:uid="{100D7B82-E1EB-4D5E-BF3E-3FAD30D873C6}"/>
+    <hyperlink ref="D2" r:id="rId2" xr:uid="{14217F5C-A074-4988-9DF3-24361DD0821E}"/>
+    <hyperlink ref="D4" r:id="rId3" xr:uid="{2A72BA92-5718-4EB3-BB32-24A7B83C698D}"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>